<commit_message>
IDEFICS-1 DPE new attempt
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_IDEFICS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_IDEFICS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5F87EF-C41A-4663-8C92-3EC43CF6B0B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CCAD57CC-B1E3-42EB-AA6F-5642678A746A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="409">
   <si>
     <t>index</t>
   </si>
@@ -1202,9 +1202,6 @@
       </rPr>
       <t>*L47)</t>
     </r>
-  </si>
-  <si>
-    <t>impossibe</t>
   </si>
   <si>
     <r>
@@ -2551,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2654,7 @@
         <v>359</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>256</v>
@@ -2683,7 +2680,7 @@
         <v>348</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>348</v>
@@ -2745,7 +2742,7 @@
         <v>348</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>348</v>
@@ -2775,7 +2772,7 @@
         <v>348</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>348</v>
@@ -2805,7 +2802,7 @@
         <v>348</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>348</v>
@@ -2835,7 +2832,7 @@
         <v>348</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>348</v>
@@ -2865,7 +2862,7 @@
         <v>348</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>348</v>
@@ -2895,7 +2892,7 @@
         <v>348</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>348</v>
@@ -2925,7 +2922,7 @@
         <v>348</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>348</v>
@@ -2955,7 +2952,7 @@
         <v>348</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>348</v>
@@ -3020,10 +3017,10 @@
         <v>258</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>256</v>
@@ -3049,7 +3046,7 @@
         <v>348</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>348</v>
@@ -3175,7 +3172,7 @@
         <v>348</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>348</v>
@@ -3208,10 +3205,10 @@
         <v>258</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>274</v>
@@ -3243,7 +3240,7 @@
         <v>254</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J22" s="18" t="s">
         <v>256</v>
@@ -3272,7 +3269,7 @@
         <v>258</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>277</v>
@@ -3336,7 +3333,7 @@
         <v>258</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>281</v>
@@ -3362,16 +3359,16 @@
         <v>355</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>258</v>
       </c>
       <c r="H26" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>373</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>374</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>274</v>
@@ -3426,16 +3423,16 @@
         <v>355</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>258</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>256</v>
@@ -3464,7 +3461,7 @@
         <v>258</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I29" s="16" t="s">
         <v>286</v>
@@ -3575,7 +3572,7 @@
         <v>348</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>348</v>
@@ -3608,10 +3605,10 @@
         <v>258</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>256</v>
@@ -3637,7 +3634,7 @@
         <v>348</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>348</v>
@@ -3670,10 +3667,10 @@
         <v>258</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>256</v>
@@ -3734,7 +3731,7 @@
         <v>258</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>295</v>
@@ -3766,7 +3763,7 @@
         <v>258</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>296</v>
@@ -3827,7 +3824,7 @@
         <v>348</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>348</v>
@@ -3857,7 +3854,7 @@
         <v>348</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>348</v>
@@ -3890,10 +3887,10 @@
         <v>258</v>
       </c>
       <c r="H42" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>375</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>376</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>256</v>
@@ -3951,7 +3948,7 @@
         <v>348</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>348</v>
@@ -3981,7 +3978,7 @@
         <v>348</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>348</v>
@@ -4011,7 +4008,7 @@
         <v>348</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>348</v>
@@ -4041,7 +4038,7 @@
         <v>348</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>348</v>
@@ -4071,7 +4068,7 @@
         <v>348</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>348</v>
@@ -4101,7 +4098,7 @@
         <v>348</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>348</v>
@@ -4163,7 +4160,7 @@
         <v>348</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>348</v>
@@ -4193,7 +4190,7 @@
         <v>348</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>348</v>
@@ -4223,7 +4220,7 @@
         <v>348</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>348</v>
@@ -4253,7 +4250,7 @@
         <v>348</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>348</v>
@@ -4283,7 +4280,7 @@
         <v>348</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>348</v>
@@ -4316,7 +4313,7 @@
         <v>258</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I56" s="10" t="s">
         <v>305</v>
@@ -4348,7 +4345,7 @@
         <v>258</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I57" s="10" t="s">
         <v>305</v>
@@ -4444,10 +4441,10 @@
         <v>258</v>
       </c>
       <c r="H60" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="I60" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="J60" s="8" t="s">
         <v>256</v>
@@ -4476,7 +4473,7 @@
         <v>258</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I61" s="10" t="s">
         <v>311</v>
@@ -4508,7 +4505,7 @@
         <v>258</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I62" s="10" t="s">
         <v>311</v>
@@ -4572,10 +4569,10 @@
         <v>258</v>
       </c>
       <c r="H64" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="I64" s="7" t="s">
         <v>382</v>
-      </c>
-      <c r="I64" s="7" t="s">
-        <v>383</v>
       </c>
       <c r="J64" s="7" t="s">
         <v>256</v>
@@ -4598,16 +4595,16 @@
         <v>355</v>
       </c>
       <c r="F65" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="I65" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>256</v>
@@ -4636,7 +4633,7 @@
         <v>258</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I66" s="12" t="s">
         <v>315</v>
@@ -4700,10 +4697,10 @@
         <v>258</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J68" s="13" t="s">
         <v>274</v>
@@ -4761,7 +4758,7 @@
         <v>348</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H70" s="15" t="s">
         <v>348</v>
@@ -4791,7 +4788,7 @@
         <v>348</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H71" s="15" t="s">
         <v>348</v>
@@ -4824,10 +4821,10 @@
         <v>258</v>
       </c>
       <c r="H72" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="I72" s="8" t="s">
         <v>388</v>
-      </c>
-      <c r="I72" s="8" t="s">
-        <v>389</v>
       </c>
       <c r="J72" s="13" t="s">
         <v>274</v>
@@ -4981,7 +4978,7 @@
         <v>348</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H77" s="15" t="s">
         <v>348</v>
@@ -5011,7 +5008,7 @@
         <v>348</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H78" s="15" t="s">
         <v>348</v>
@@ -5044,10 +5041,10 @@
         <v>258</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J79" s="11" t="s">
         <v>274</v>
@@ -5076,10 +5073,10 @@
         <v>258</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J80" s="11" t="s">
         <v>274</v>
@@ -5108,10 +5105,10 @@
         <v>258</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J81" s="11" t="s">
         <v>274</v>
@@ -5169,7 +5166,7 @@
         <v>348</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H83" s="15" t="s">
         <v>348</v>
@@ -5199,7 +5196,7 @@
         <v>348</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H84" s="15" t="s">
         <v>348</v>
@@ -5232,10 +5229,10 @@
         <v>258</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I85" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J85" s="14" t="s">
         <v>256</v>
@@ -5267,7 +5264,7 @@
         <v>254</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>256</v>
@@ -5299,7 +5296,7 @@
         <v>254</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>256</v>
@@ -5331,7 +5328,7 @@
         <v>254</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>256</v>
@@ -5357,7 +5354,7 @@
         <v>348</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H89" s="15" t="s">
         <v>348</v>
@@ -5387,7 +5384,7 @@
         <v>348</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H90" s="15" t="s">
         <v>348</v>
@@ -5417,7 +5414,7 @@
         <v>348</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H91" s="15" t="s">
         <v>348</v>
@@ -5447,7 +5444,7 @@
         <v>348</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H92" s="15" t="s">
         <v>348</v>
@@ -5573,7 +5570,7 @@
         <v>348</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H96" s="15" t="s">
         <v>348</v>
@@ -5635,7 +5632,7 @@
         <v>348</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H98" s="15" t="s">
         <v>348</v>
@@ -5665,7 +5662,7 @@
         <v>348</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H99" s="15" t="s">
         <v>348</v>
@@ -5695,7 +5692,7 @@
         <v>348</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H100" s="15" t="s">
         <v>348</v>
@@ -5725,7 +5722,7 @@
         <v>348</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H101" s="15" t="s">
         <v>348</v>
@@ -5787,7 +5784,7 @@
         <v>348</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H103" s="15" t="s">
         <v>348</v>
@@ -5817,7 +5814,7 @@
         <v>348</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H104" s="15" t="s">
         <v>348</v>
@@ -5847,7 +5844,7 @@
         <v>348</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H105" s="15" t="s">
         <v>348</v>
@@ -5877,7 +5874,7 @@
         <v>348</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H106" s="15" t="s">
         <v>348</v>
@@ -5907,7 +5904,7 @@
         <v>348</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H107" s="15" t="s">
         <v>348</v>
@@ -5937,7 +5934,7 @@
         <v>348</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H108" s="15" t="s">
         <v>348</v>
@@ -5967,7 +5964,7 @@
         <v>348</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H109" s="15" t="s">
         <v>348</v>
@@ -5997,7 +5994,7 @@
         <v>348</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H110" s="15" t="s">
         <v>348</v>
@@ -6030,7 +6027,7 @@
         <v>258</v>
       </c>
       <c r="H111" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I111" s="3" t="s">
         <v>347</v>
@@ -6059,7 +6056,7 @@
         <v>348</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H112" s="15" t="s">
         <v>348</v>
@@ -6089,7 +6086,7 @@
         <v>348</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H113" s="15" t="s">
         <v>348</v>
@@ -6119,7 +6116,7 @@
         <v>348</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H114" s="15" t="s">
         <v>348</v>
@@ -6178,7 +6175,7 @@
         <v>355</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>254</v>
@@ -6187,7 +6184,7 @@
         <v>254</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J116" s="3" t="s">
         <v>256</v>
@@ -6213,7 +6210,7 @@
         <v>348</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H117" s="15" t="s">
         <v>348</v>
@@ -6243,7 +6240,7 @@
         <v>348</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H118" s="15" t="s">
         <v>348</v>
@@ -6273,7 +6270,7 @@
         <v>348</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H119" s="15" t="s">
         <v>348</v>
@@ -6303,7 +6300,7 @@
         <v>348</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="H120" s="15" t="s">
         <v>348</v>
@@ -6339,7 +6336,7 @@
         <v>2</v>
       </c>
       <c r="I121" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J121" s="3" t="s">
         <v>256</v>

</xml_diff>